<commit_message>
*SysSettings.xlsx* - Runfile Switches: -Report value flows by process -Activiate levelised cost calculation -Split investment according to hurdle rate
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Training material\DemoS_012\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kristoffer\DemoS_012_timesreport\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B7052D-B7CA-4120-BF32-6D58CA11CCA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB81F9BC-5412-43B2-B774-C6A9A603758B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="853" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -20,19 +20,25 @@
     <sheet name="Constants" sheetId="20" r:id="rId5"/>
     <sheet name="Defaults" sheetId="21" r:id="rId6"/>
     <sheet name="Commodity Group" sheetId="15" r:id="rId7"/>
+    <sheet name="Runfile Switches" sheetId="23" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -126,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -435,6 +441,57 @@
   </si>
   <si>
     <t>Year2</t>
+  </si>
+  <si>
+    <t>Switch</t>
+  </si>
+  <si>
+    <t>FLO~1</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Report Value flows at commodity TS level</t>
+  </si>
+  <si>
+    <t>FLO~3</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Report value flows by process</t>
+  </si>
+  <si>
+    <t>FLO~5</t>
+  </si>
+  <si>
+    <t>Report electricity supply by energy source</t>
+  </si>
+  <si>
+    <t>FLO~7</t>
+  </si>
+  <si>
+    <t>Report process topology indicators</t>
+  </si>
+  <si>
+    <t>COMPRD~1</t>
+  </si>
+  <si>
+    <t>Report VAR_COMPRD for all commodities</t>
+  </si>
+  <si>
+    <t>NCAP~1</t>
+  </si>
+  <si>
+    <t>Activiate levelised cost calculation</t>
+  </si>
+  <si>
+    <t>OBJ~1</t>
+  </si>
+  <si>
+    <t>Split investment according to hurdle rate</t>
   </si>
 </sst>
 </file>
@@ -442,10 +499,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -534,6 +591,12 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -795,23 +858,22 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -823,19 +885,15 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -860,20 +918,18 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -883,13 +939,13 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -898,7 +954,7 @@
     <xf numFmtId="2" fontId="13" fillId="4" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -913,23 +969,23 @@
     <xf numFmtId="2" fontId="13" fillId="4" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -941,9 +997,6 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -953,16 +1006,14 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Migliaia_tab emissioni" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2949,8 +3000,57 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>487680</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>118588</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>29685</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Billede 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54D52C9C-9FCC-42D2-923F-4F7676ADF948}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6583680" y="617220"/>
+          <a:ext cx="5726908" cy="2088990"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="IEA Data"/>
@@ -3085,9 +3185,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3125,9 +3225,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3160,26 +3260,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3212,26 +3295,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3405,7 +3471,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:J38"/>
+  <dimension ref="B3:J6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -3418,8 +3484,7 @@
     <col min="8" max="8" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3429,8 +3494,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
@@ -3447,159 +3511,33 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="17" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="77" t="s">
+      <c r="C6" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" t="s">
         <v>81</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
+      <c r="J6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -3653,104 +3591,104 @@
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="79" t="s">
+      <c r="C12" s="67" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="80" t="s">
+      <c r="D12" s="68" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="16">
+      <c r="B13" s="15">
         <v>1</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>1</v>
       </c>
-      <c r="D13" s="16">
+      <c r="D13" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B14" s="16">
+      <c r="B14" s="15">
         <v>2</v>
       </c>
-      <c r="C14" s="16">
+      <c r="C14" s="15">
         <v>2</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D14" s="15">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="16"/>
-      <c r="C15" s="16">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15">
         <v>5</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="16"/>
-      <c r="C16" s="16">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15">
         <v>5</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D16" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B17" s="16"/>
-      <c r="C17" s="16">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15">
         <v>5</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D17" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B18" s="16"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B22" s="16"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15">
         <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15">
         <v>5</v>
       </c>
     </row>
@@ -3776,71 +3714,71 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="63" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:3" s="73" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="75" t="s">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="64" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="75">
+      <c r="C5" s="64">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="76" t="s">
+      <c r="B6" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="16">
+      <c r="C8" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C9" s="16">
+      <c r="C9" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>0</v>
       </c>
     </row>
@@ -3857,7 +3795,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B3:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -3915,10 +3853,10 @@
       <c r="C6" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E6" s="20">
+      <c r="E6" s="16">
         <v>0</v>
       </c>
       <c r="F6">
@@ -3929,10 +3867,10 @@
       <c r="C7" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E7" s="20">
+      <c r="E7" s="16">
         <v>0</v>
       </c>
       <c r="F7">
@@ -3942,16 +3880,16 @@
     <row r="18" spans="2:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
@@ -4012,13 +3950,9 @@
       <c r="D35" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6">
+      <c r="G35">
         <v>2222</v>
       </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
       <c r="J35" t="s">
         <v>18</v>
       </c>
@@ -4030,13 +3964,9 @@
       <c r="D36" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6">
+      <c r="G36">
         <v>8888</v>
       </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
       <c r="J36" t="s">
         <v>18</v>
       </c>
@@ -4057,26 +3987,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B3:H33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="12.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="12.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -4104,73 +4036,65 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="11">
         <v>2005</v>
       </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="11">
         <v>0.05</v>
       </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="72">
+      <c r="E9" s="17">
         <f>C23</f>
         <v>0.24971461187214614</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="71" t="s">
+      <c r="B10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="72">
+      <c r="E10" s="17">
         <f>D23</f>
         <v>0.22973744292237441</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="71" t="s">
+      <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="71"/>
-      <c r="D11" s="71" t="s">
+      <c r="D11" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="72">
+      <c r="E11" s="17">
         <f>E23</f>
         <v>0.24942922374429224</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="71" t="s">
+      <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="71"/>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="72">
+      <c r="E12" s="17">
         <f>F23</f>
         <v>0.27111872146118721</v>
       </c>
@@ -4178,265 +4102,248 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13"/>
       <c r="C13"/>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19">
+      <c r="F13" s="17">
         <v>0.9</v>
       </c>
-      <c r="G13" s="19">
+      <c r="G13" s="17">
         <v>0.95</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="H13" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14"/>
       <c r="C14"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
     </row>
     <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="C19" s="23"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="26" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.2">
-      <c r="B22" s="32"/>
-      <c r="C22" s="33" t="s">
+      <c r="B22" s="27"/>
+      <c r="C22" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="34" t="s">
+      <c r="E22" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="35" t="s">
+      <c r="F22" s="30" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="36">
+      <c r="C23" s="31">
         <f>C32/$F32*$E27</f>
         <v>0.24971461187214614</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="32">
         <f>D32/$F32*$E27</f>
         <v>0.22973744292237441</v>
       </c>
-      <c r="E23" s="37">
+      <c r="E23" s="32">
         <f>C33/$F33*$E28</f>
         <v>0.24942922374429224</v>
       </c>
-      <c r="F23" s="38">
+      <c r="F23" s="33">
         <f>D33/$F33*$E28</f>
         <v>0.27111872146118721</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="34">
         <f>SUM(C23:F23)</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="41"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="40"/>
-      <c r="G25" s="43"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="44" t="s">
+      <c r="B26" s="35"/>
+      <c r="C26" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="F26" s="47"/>
-      <c r="G26" s="43"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="35"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="49" t="s">
+      <c r="C27" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="50">
+      <c r="D27" s="43">
         <v>175</v>
       </c>
-      <c r="E27" s="51">
+      <c r="E27" s="44">
         <f>D27/D29</f>
         <v>0.47945205479452052</v>
       </c>
-      <c r="F27" s="52"/>
-      <c r="G27" s="43"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="35"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B28" s="53" t="s">
+      <c r="B28" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="47" t="s">
         <v>78</v>
       </c>
-      <c r="D28" s="55">
+      <c r="D28" s="48">
         <f>365-D27</f>
         <v>190</v>
       </c>
-      <c r="E28" s="56">
+      <c r="E28" s="49">
         <f>D28/D29</f>
         <v>0.52054794520547942</v>
       </c>
-      <c r="F28" s="52"/>
-      <c r="G28" s="43"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="35"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B29" s="41"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="57">
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="50">
         <f>SUM(D27:D28)</f>
         <v>365</v>
       </c>
-      <c r="E29" s="58">
+      <c r="E29" s="51">
         <f>SUM(E27:E28)</f>
         <v>1</v>
       </c>
-      <c r="F29" s="59"/>
-      <c r="G29" s="43"/>
+      <c r="F29" s="52"/>
+      <c r="G29" s="35"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B30" s="41"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="43"/>
-      <c r="G30" s="43"/>
+      <c r="B30" s="35"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B31" s="61"/>
-      <c r="C31" s="62" t="s">
+      <c r="B31" s="54"/>
+      <c r="C31" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D31" s="46" t="s">
+      <c r="D31" s="39" t="s">
         <v>80</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B32" s="64" t="s">
+      <c r="B32" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="C32" s="65">
+      <c r="C32" s="58">
         <v>12.5</v>
       </c>
-      <c r="D32" s="66">
+      <c r="D32" s="59">
         <v>11.5</v>
       </c>
-      <c r="E32" s="59"/>
-      <c r="F32" s="67">
+      <c r="E32" s="52"/>
+      <c r="F32" s="52">
         <f>SUM(C32:E32)</f>
         <v>24</v>
       </c>
-      <c r="G32" s="43"/>
+      <c r="G32" s="35"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="C33" s="69">
+      <c r="C33" s="61">
         <v>11.5</v>
       </c>
-      <c r="D33" s="70">
+      <c r="D33" s="62">
         <v>12.5</v>
       </c>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59">
+      <c r="E33" s="52"/>
+      <c r="F33" s="52">
         <f>SUM(C33:E33)</f>
         <v>24</v>
       </c>
-      <c r="G33" s="43"/>
+      <c r="G33" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4449,7 +4356,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4472,74 +4379,72 @@
       </c>
     </row>
     <row r="3" spans="2:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="H3" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="18" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="16" t="s">
         <v>98</v>
       </c>
       <c r="D4" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="20" t="s">
+      <c r="H4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="6"/>
       <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="20" t="s">
+      <c r="F5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="16" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="6"/>
       <c r="D6" t="s">
         <v>54</v>
       </c>
@@ -4555,12 +4460,9 @@
       <c r="H6" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="17" t="s">
+      <c r="I6" s="16" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4571,9 +4473,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:I7"/>
+  <dimension ref="B2:I7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4586,34 +4490,25 @@
     <col min="9" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
     <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -4647,18 +4542,18 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -4667,4 +4562,175 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CF077CF-BCE9-46D4-AD95-5EB6BFB2C2E4}">
+  <dimension ref="B3:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="70" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="70" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="G4" s="70" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="69" t="str">
+        <f t="shared" ref="B5:B11" si="0">IF(F5="Yes","RPT_OPT","*")</f>
+        <v>*</v>
+      </c>
+      <c r="C5" s="69" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="69">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>RPT_OPT</v>
+      </c>
+      <c r="C6" s="69" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" s="69">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+      <c r="C7" s="69" t="s">
+        <v>110</v>
+      </c>
+      <c r="D7" s="69">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+      <c r="C8" s="69" t="s">
+        <v>112</v>
+      </c>
+      <c r="D8" s="69">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>*</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>114</v>
+      </c>
+      <c r="D9" s="69">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>RPT_OPT</v>
+      </c>
+      <c r="C10" s="69" t="s">
+        <v>116</v>
+      </c>
+      <c r="D10" s="69">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="69" t="str">
+        <f t="shared" si="0"/>
+        <v>RPT_OPT</v>
+      </c>
+      <c r="C11" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="69">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>108</v>
+      </c>
+      <c r="G11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>